<commit_message>
committing another test suite
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC02_CCDI_phs002504_Sex-Female_Race-Unknown_Trt-Chemotherapy.xlsx
+++ b/InputFiles/CCDI/TC02_CCDI_phs002504_Sex-Female_Race-Unknown_Trt-Chemotherapy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation\sowjanya0417\Commons_Automation\InputFiles\CCDI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatekaraa\Automation\06-05-25\Commons_Automation\InputFiles\CCDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D86A454-BC75-44C2-8FBB-E8E89A6F02C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8C86CE-9102-400F-A4D6-33C3389CB377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -290,19 +290,21 @@
     COUNT(DISTINCT std.dbgap_accession) AS "Studies",
     COUNT(DISTINCT prt.participant_id) AS "Participants",
     COUNT(DISTINCT smp.sample_id) AS "Samples",
-    (COUNT(DISTINCT maf.methylation_array_file_id) ) AS "Files"
+    (COUNT(DISTINCT seq.sequencing_file_id) + COUNT(DISTINCT maf.methylation_array_file_id)) AS "Files"
 FROM 
     df_study std
 LEFT JOIN df_participant prt ON std.id = prt."study.id"
 LEFT JOIN df_sample smp ON prt.id = smp."participant.id"
-LEFT JOIN df_treatment trt ON prt.id = trt."participant.id"
+LEFT JOIN df_diagnosis dgn ON prt.id = dgn."participant.id"
+LEFT JOIN df_survival srv ON prt.id = srv."participant.id"
+LEFT JOIN df_sequencing_file seq ON smp.id = seq."sample.id"
+LEFT JOIN df_treatment  trt ON prt.id = trt."participant_id"
 LEFT JOIN df_methylation_array_file maf ON smp.id = maf."sample.id"
 WHERE 
-    std.dbgap_accession = 'phs002504'
-    AND prt.sex_at_birth = 'Female'
-    AND prt.race = 'Unknown'
-    AND trt.treatment_type LIKE '%Chemotherapy%'
-     ;</t>
+std.dbgap_accession = 'phs002504' 
+AND prt.sex_at_birth = 'Female'
+AND prt.race = 'Unknown'
+AND trt.treatment_type LIKE '%Chemotherapy%';</t>
   </si>
 </sst>
 </file>

</xml_diff>